<commit_message>
Exercise 2.B NorthwindTablesAndColumns Excel file
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reliablecollaboration-my.sharepoint.com/personal/bess_rcc_team/Documents/Courseware/DataAnalyticsWeek5-8/Student Files/Week 9 downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\Week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA878EF4-4B80-439A-88BC-05CECC90D1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B4FAAC-8EC6-4414-AD35-9874422EDC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Northwind Columns" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="158">
   <si>
     <t>table_name</t>
   </si>
@@ -308,13 +308,214 @@
   </si>
   <si>
     <t>New Name?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes </t>
+  </si>
+  <si>
+    <t>for category name space needs to added and we might need space or and for this "/".</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>because title might not be needed for aggregating</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Employee Title</t>
+  </si>
+  <si>
+    <t>Employee Region</t>
+  </si>
+  <si>
+    <t>Employee Country</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for first and last name we might need to concate in one column as name </t>
+  </si>
+  <si>
+    <t>I this might be use full with names and what does he do in the company</t>
+  </si>
+  <si>
+    <t>for calcualting the age of employees</t>
+  </si>
+  <si>
+    <t>to calculate how long an employee worked for</t>
+  </si>
+  <si>
+    <t>I decided to keep this it is a important information to keep track.</t>
+  </si>
+  <si>
+    <t>EmployeeTerritories they are redunanat data</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Employee Birth Date</t>
+  </si>
+  <si>
+    <t>Employee Hire Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee City </t>
+  </si>
+  <si>
+    <t>Employee Postal Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customers City </t>
+  </si>
+  <si>
+    <t>Customers Region</t>
+  </si>
+  <si>
+    <t>Customers Postal Code</t>
+  </si>
+  <si>
+    <t>Customers Country</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Contact </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Customer Contact Title</t>
+  </si>
+  <si>
+    <t>Employee Title Of Courtesy</t>
+  </si>
+  <si>
+    <t>EmployeeReportsToEmployeeId</t>
+  </si>
+  <si>
+    <t>Sales Quantity</t>
+  </si>
+  <si>
+    <t>Sales Discount Percent</t>
+  </si>
+  <si>
+    <t>Order Required Date</t>
+  </si>
+  <si>
+    <t>Order Shipped Date</t>
+  </si>
+  <si>
+    <t>Order Freight Amount</t>
+  </si>
+  <si>
+    <t>Order Ship Name</t>
+  </si>
+  <si>
+    <t>Order Ship City</t>
+  </si>
+  <si>
+    <t>Order Ship Region</t>
+  </si>
+  <si>
+    <t>Order Ship Postal Code</t>
+  </si>
+  <si>
+    <t>Order Ship Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Product Current Unit Price</t>
+  </si>
+  <si>
+    <t>Product Units In Stock</t>
+  </si>
+  <si>
+    <t>Product Units On Order</t>
+  </si>
+  <si>
+    <t>Product Reorder Level</t>
+  </si>
+  <si>
+    <t>Product Discontinued</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Supplier Contact</t>
+  </si>
+  <si>
+    <t>Supplier Contact Title</t>
+  </si>
+  <si>
+    <t>Supplier City</t>
+  </si>
+  <si>
+    <t>Supplier Region</t>
+  </si>
+  <si>
+    <t>Supplier Postal Code</t>
+  </si>
+  <si>
+    <t>Supplier Country</t>
+  </si>
+  <si>
+    <t>Territory</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Sales Amount, Discount Amount</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Discount Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,8 +530,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +563,36 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -371,11 +609,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -394,6 +647,29 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1064EA23-634A-4960-9ACD-6B0F910F333B}" name="Table1" displayName="Table1" ref="A1:N85" totalsRowShown="0" headerRowCellStyle="20% - Accent1">
+  <autoFilter ref="A1:N85" xr:uid="{1064EA23-634A-4960-9ACD-6B0F910F333B}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{EA0B16AE-26D2-4499-942F-F122CBB2BF03}" name="table_name" dataCellStyle="20% - Accent2"/>
+    <tableColumn id="2" xr3:uid="{162D97AF-B46B-44C1-A3EF-B77C218BE84D}" name="column_id" dataCellStyle="20% - Accent2"/>
+    <tableColumn id="3" xr3:uid="{E538B605-DB42-45D7-9691-D45D6CCE1FE8}" name="column_name" dataCellStyle="20% - Accent2"/>
+    <tableColumn id="4" xr3:uid="{8A4915B5-F874-4389-B383-5A21BC5D83D2}" name="data_type" dataCellStyle="20% - Accent2"/>
+    <tableColumn id="5" xr3:uid="{82C7DFDB-0E29-4383-8C18-40D8E3F16E87}" name="max_length" dataCellStyle="20% - Accent2"/>
+    <tableColumn id="6" xr3:uid="{AA2CD5E7-F20A-49A5-B907-B9ED0E3D857A}" name="Primary Key?"/>
+    <tableColumn id="7" xr3:uid="{88D37C82-3FBC-4E88-AE25-BDD6143B40DB}" name="Foreign Key?"/>
+    <tableColumn id="8" xr3:uid="{D6322846-F7EB-4E4F-B966-50D33587DB12}" name="Keep it?"/>
+    <tableColumn id="9" xr3:uid="{ACA907CB-58EF-43D5-8DED-6E8C5D779BDB}" name="New Name?"/>
+    <tableColumn id="10" xr3:uid="{E16E169B-5EA0-445D-87A1-0FE7A58027C3}" name="Measure Candidate?"/>
+    <tableColumn id="11" xr3:uid="{CBBABC79-1953-47D3-8F52-97F146F21336}" name="Attribute Candidate?"/>
+    <tableColumn id="12" xr3:uid="{56C5DC8B-77A6-4A3D-9008-EF7F89AD5BFC}" name="Formatting Considerations?"/>
+    <tableColumn id="13" xr3:uid="{2F65765A-21E4-4A85-B534-D74E173DCA36}" name="Calculations?"/>
+    <tableColumn id="14" xr3:uid="{FC60F6E2-486A-4BC7-9176-50F3DF3BB5C7}" name="Notes:"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,27 +971,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B56A5E-AA28-4DB9-BAE3-51DE131C631E}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" customWidth="1"/>
-    <col min="2" max="2" width="10.265625" customWidth="1"/>
-    <col min="3" max="3" width="17.1328125" customWidth="1"/>
-    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.265625" customWidth="1"/>
-    <col min="7" max="7" width="17.86328125" customWidth="1"/>
-    <col min="9" max="9" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.59765625" customWidth="1"/>
-    <col min="13" max="13" width="11.59765625" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="72.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +1038,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -775,8 +1054,25 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -792,8 +1088,29 @@
       <c r="E3" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -809,8 +1126,19 @@
       <c r="E4" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -826,8 +1154,19 @@
       <c r="E5" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -843,8 +1182,27 @@
       <c r="E6" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -860,8 +1218,23 @@
       <c r="E7" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -877,8 +1250,27 @@
       <c r="E8" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -894,8 +1286,25 @@
       <c r="E9" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -911,8 +1320,19 @@
       <c r="E10" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -928,8 +1348,24 @@
       <c r="E11" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="H11" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -945,8 +1381,24 @@
       <c r="E12" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="H12" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -962,8 +1414,24 @@
       <c r="E13" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="H13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -979,8 +1447,24 @@
       <c r="E14" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="H14" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -996,8 +1480,11 @@
       <c r="E15" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="H15" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1013,8 +1500,11 @@
       <c r="E16" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H16" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1030,8 +1520,28 @@
       <c r="E17" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1047,8 +1557,27 @@
       <c r="E18" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H18" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1064,8 +1593,24 @@
       <c r="E19" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H19" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1081,8 +1626,27 @@
       <c r="E20" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H20" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1098,8 +1662,17 @@
       <c r="E21" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H21" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1115,8 +1688,26 @@
       <c r="E22" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H22" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1132,8 +1723,26 @@
       <c r="E23" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H23" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1149,8 +1758,11 @@
       <c r="E24" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H24" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1166,8 +1778,23 @@
       <c r="E25" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H25" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1183,8 +1810,23 @@
       <c r="E26" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H26" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1200,8 +1842,23 @@
       <c r="E27" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H27" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1217,8 +1874,23 @@
       <c r="E28" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H28" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1234,8 +1906,11 @@
       <c r="E29" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H29" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1251,8 +1926,11 @@
       <c r="E30" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H30" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1268,8 +1946,11 @@
       <c r="E31" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H31" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1285,8 +1966,11 @@
       <c r="E32" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H32" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1302,8 +1986,21 @@
       <c r="E33" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G33" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="K33" s="5"/>
+      <c r="N33" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1319,8 +2016,11 @@
       <c r="E34" s="1">
         <v>510</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H34" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -1336,8 +2036,20 @@
       <c r="E35" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F35" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -1353,8 +2065,20 @@
       <c r="E36" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F36" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -1370,8 +2094,27 @@
       <c r="E37" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1387,8 +2130,27 @@
       <c r="E38" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F38" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K38" s="13"/>
+      <c r="L38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1404,8 +2166,25 @@
       <c r="E39" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H39" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="M39" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N39" s="16"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1421,8 +2200,25 @@
       <c r="E40" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H40" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K40" s="15"/>
+      <c r="L40" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N40" s="16"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1438,8 +2234,25 @@
       <c r="E41" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H41" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K41" s="15"/>
+      <c r="L41" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="M41" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N41" s="16"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -1455,8 +2268,26 @@
       <c r="E42" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="6"/>
+      <c r="H42" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -1472,8 +2303,23 @@
       <c r="E43" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G43" s="5"/>
+      <c r="H43" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M43" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -1489,8 +2335,15 @@
       <c r="E44" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G44" s="5"/>
+      <c r="H44" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>53</v>
       </c>
@@ -1506,8 +2359,20 @@
       <c r="E45" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H45" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="K45" t="s">
+        <v>139</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1523,8 +2388,20 @@
       <c r="E46" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H46" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="K46" t="s">
+        <v>139</v>
+      </c>
+      <c r="L46" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -1540,8 +2417,20 @@
       <c r="E47" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H47" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="K47" t="s">
+        <v>91</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -1557,8 +2446,18 @@
       <c r="E48" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G48" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="L48" s="16"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -1574,8 +2473,20 @@
       <c r="E49" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H49" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I49" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="J49" t="s">
+        <v>91</v>
+      </c>
+      <c r="L49" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -1591,8 +2502,17 @@
       <c r="E50" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H50" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="K50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -1608,8 +2528,11 @@
       <c r="E51" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H51" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -1625,8 +2548,14 @@
       <c r="E52" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H52" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I52" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -1642,8 +2571,14 @@
       <c r="E53" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H53" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I53" s="17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -1659,8 +2594,14 @@
       <c r="E54" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H54" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -1676,8 +2617,14 @@
       <c r="E55" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H55" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I55" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1693,8 +2640,11 @@
       <c r="E56" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H56" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -1710,8 +2660,14 @@
       <c r="E57" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H57" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1727,8 +2683,14 @@
       <c r="E58" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G58" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -1744,8 +2706,14 @@
       <c r="E59" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G59" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1761,8 +2729,11 @@
       <c r="E60" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H60" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -1778,8 +2749,23 @@
       <c r="E61" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H61" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K61" t="s">
+        <v>139</v>
+      </c>
+      <c r="L61" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -1795,8 +2781,23 @@
       <c r="E62" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H62" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K62" t="s">
+        <v>91</v>
+      </c>
+      <c r="L62" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -1812,8 +2813,23 @@
       <c r="E63" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H63" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I63" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K63" t="s">
+        <v>139</v>
+      </c>
+      <c r="L63" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -1829,8 +2845,23 @@
       <c r="E64" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H64" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I64" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K64" t="s">
+        <v>139</v>
+      </c>
+      <c r="L64" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -1846,8 +2877,20 @@
       <c r="E65" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H65" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I65" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K65" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>22</v>
       </c>
@@ -1863,8 +2906,14 @@
       <c r="E66" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F66" t="s">
+        <v>91</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -1880,8 +2929,14 @@
       <c r="E67" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H67" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -1897,8 +2952,14 @@
       <c r="E68" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F68" t="s">
+        <v>91</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>76</v>
       </c>
@@ -1914,8 +2975,11 @@
       <c r="E69" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H69" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -1931,8 +2995,11 @@
       <c r="E70" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H70" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>78</v>
       </c>
@@ -1948,8 +3015,14 @@
       <c r="E71" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F71" t="s">
+        <v>91</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -1965,8 +3038,17 @@
       <c r="E72" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H72" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I72" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="K72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -1982,8 +3064,17 @@
       <c r="E73" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H73" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I73" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="K73" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -1999,8 +3090,17 @@
       <c r="E74" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H74" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I74" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="K74" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
@@ -2016,8 +3116,12 @@
       <c r="E75" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H75" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I75" s="16"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -2033,8 +3137,17 @@
       <c r="E76" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H76" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="K76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -2050,8 +3163,17 @@
       <c r="E77" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H77" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I77" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="K77" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -2067,8 +3189,17 @@
       <c r="E78" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H78" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I78" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="K78" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2084,8 +3215,17 @@
       <c r="E79" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H79" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I79" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="K79" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -2101,8 +3241,12 @@
       <c r="E80" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H80" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I80" s="16"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
@@ -2118,8 +3262,12 @@
       <c r="E81" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H81" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I81" s="16"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -2135,8 +3283,12 @@
       <c r="E82" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H82" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I82" s="16"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2152,8 +3304,15 @@
       <c r="E83" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F83" t="s">
+        <v>91</v>
+      </c>
+      <c r="H83" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I83" s="16"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>80</v>
       </c>
@@ -2169,8 +3328,17 @@
       <c r="E84" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H84" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I84" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="K84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
@@ -2186,9 +3354,18 @@
       <c r="E85" s="1">
         <v>4</v>
       </c>
+      <c r="G85" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2202,6 +3379,25 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA5D0A6329BB324E86983B32928CFC2E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b28f3bc5995c0091f528145aa367664">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xmlns:ns3="ced60a7f-99b1-48d2-b555-34851c8026ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48800952b0413791e1a5c8543532e00d" ns2:_="" ns3:_="">
     <xsd:import namespace="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
@@ -2442,25 +3638,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
   <ds:schemaRefs>
@@ -2470,6 +3647,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
+    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F2F57-CFBB-4DE2-9688-0C0C6A435162}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2486,15 +3674,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
-    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>